<commit_message>
Preview single file and docrumets structure
</commit_message>
<xml_diff>
--- a/documents/crated_models.xlsx
+++ b/documents/crated_models.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\PCGClassification\PCGTransformer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\PCGClassification\PCGTransformer\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5280C8D0-CF98-4FF3-979A-BF2A5DCED685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD2DB98-AC1E-412C-B973-14B49B4BDE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="44">
   <si>
     <t>Dataset</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>Schlecht recall, Instabil</t>
+  </si>
+  <si>
+    <t>OUTDATED</t>
   </si>
 </sst>
 </file>
@@ -1082,7 +1085,7 @@
   <dimension ref="A2:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="D30:E30"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1589,7 +1592,9 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F29" s="35"/>
-      <c r="G29" s="35"/>
+      <c r="G29" s="35" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F30" s="35"/>

</xml_diff>